<commit_message>
updates for final manuscript
</commit_message>
<xml_diff>
--- a/Bat_morphology_SI_tables.xlsx
+++ b/Bat_morphology_SI_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caraebrook/Documents/R/R_repositories/Mada-Bat-Morphology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F64D16-01C3-B94E-B9CF-3126DA82C34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9437F737-C2C9-B04B-A839-7F863048142E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="1120" windowWidth="17280" windowHeight="14740" tabRatio="995" firstSheet="1" activeTab="7" xr2:uid="{1B6F4642-3560-4916-8B50-A310AAB2757D}"/>
+    <workbookView xWindow="11520" yWindow="1120" windowWidth="17280" windowHeight="14740" tabRatio="995" firstSheet="1" activeTab="4" xr2:uid="{1B6F4642-3560-4916-8B50-A310AAB2757D}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6885" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6892" uniqueCount="98">
   <si>
     <t>M/D/Y</t>
   </si>
@@ -330,6 +330,12 @@
   <si>
     <t>0.0073**</t>
   </si>
+  <si>
+    <t>&lt;0.01**</t>
+  </si>
+  <si>
+    <t>0.029*</t>
+  </si>
 </sst>
 </file>
 
@@ -338,7 +344,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +401,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -570,7 +583,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -630,92 +643,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -756,6 +685,100 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,72 +1107,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="63"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1183,15 +1206,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -1346,911 +1369,921 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A837B06-C918-43E5-817F-08CC4381E50D}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.1640625" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-    </row>
-    <row r="2" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="24" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+    </row>
+    <row r="3" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="91"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C4" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D4" s="25">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E4" s="26">
         <v>0.5</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F4" s="35">
         <v>0.97499999999999998</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G4" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H4" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I4" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K4" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="s">
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B5" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>21.84</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>29</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>37.96</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>20.059999999999999</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H5" s="8">
         <v>40.6</v>
       </c>
-      <c r="I4" s="54">
+      <c r="I5" s="67">
         <v>29.229457364341101</v>
       </c>
-      <c r="J4" s="54">
+      <c r="J5" s="67">
         <v>28.770814814814798</v>
       </c>
-      <c r="K4" s="58">
+      <c r="K5" s="68">
         <v>0.40963601233378399</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="9" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>20.54</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>28.7</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>37.725000000000001</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>19.399999999999999</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H6" s="9">
         <v>42.3</v>
       </c>
-      <c r="I5" s="55">
+      <c r="I6" s="64">
         <v>29.229457364341101</v>
       </c>
-      <c r="J5" s="55">
+      <c r="J6" s="64">
         <v>28.770814814814798</v>
       </c>
-      <c r="K5" s="59">
+      <c r="K6" s="66">
         <v>0.40963601233378399</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="45"/>
-      <c r="B6" s="50" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="72"/>
+      <c r="B7" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>69.143500000000003</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>79.215000000000003</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>88.732500000000002</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>61.4</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H7" s="9">
         <v>92</v>
       </c>
-      <c r="I6" s="55">
+      <c r="I7" s="64">
         <v>78.608461538461498</v>
       </c>
-      <c r="J6" s="55">
+      <c r="J7" s="64">
         <v>81.037333333333294</v>
       </c>
-      <c r="K6" s="59">
+      <c r="K7" s="66" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="72"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>67.275000000000006</v>
+      </c>
+      <c r="E8">
+        <v>81.87</v>
+      </c>
+      <c r="F8">
+        <v>92.06</v>
+      </c>
+      <c r="G8">
+        <v>56</v>
+      </c>
+      <c r="H8" s="9">
+        <v>100</v>
+      </c>
+      <c r="I8" s="64">
+        <v>78.608461538461498</v>
+      </c>
+      <c r="J8" s="64">
+        <v>81.037333333333294</v>
+      </c>
+      <c r="K8" s="66">
         <v>4.5957771759546397E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="45"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="28" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="72"/>
+      <c r="B9" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9">
+        <v>144.36000000000001</v>
+      </c>
+      <c r="E9">
+        <v>164</v>
+      </c>
+      <c r="F9">
+        <v>175</v>
+      </c>
+      <c r="G9">
+        <v>130.5</v>
+      </c>
+      <c r="H9" s="9">
+        <v>177</v>
+      </c>
+      <c r="I9" s="64">
+        <v>162.44821705426401</v>
+      </c>
+      <c r="J9" s="64">
+        <v>167.47703703703701</v>
+      </c>
+      <c r="K9" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="73"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7">
-        <v>67.275000000000006</v>
-      </c>
-      <c r="E7">
-        <v>81.87</v>
-      </c>
-      <c r="F7">
-        <v>92.06</v>
-      </c>
-      <c r="G7">
-        <v>56</v>
-      </c>
-      <c r="H7" s="9">
-        <v>100</v>
-      </c>
-      <c r="I7" s="55">
-        <v>78.608461538461498</v>
-      </c>
-      <c r="J7" s="55">
-        <v>81.037333333333294</v>
-      </c>
-      <c r="K7" s="59">
+      <c r="D10">
+        <v>145.91499999999999</v>
+      </c>
+      <c r="E10">
+        <v>169</v>
+      </c>
+      <c r="F10">
+        <v>180.65</v>
+      </c>
+      <c r="G10">
+        <v>143</v>
+      </c>
+      <c r="H10" s="9">
+        <v>191</v>
+      </c>
+      <c r="I10" s="64">
+        <v>162.44821705426401</v>
+      </c>
+      <c r="J10" s="64">
+        <v>167.47703703703701</v>
+      </c>
+      <c r="K10" s="66">
         <v>4.5957771759546397E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
-      <c r="B8" s="51" t="s">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="8">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8">
+        <v>13.5</v>
+      </c>
+      <c r="F11" s="8">
+        <v>17.647500000000001</v>
+      </c>
+      <c r="G11" s="8">
+        <v>7.1</v>
+      </c>
+      <c r="H11" s="8">
+        <v>23.93</v>
+      </c>
+      <c r="I11" s="67">
+        <v>13.6002631578947</v>
+      </c>
+      <c r="J11" s="67">
+        <v>13.0713381995134</v>
+      </c>
+      <c r="K11" s="66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="72"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>9.15</v>
+      </c>
+      <c r="E12">
+        <v>12.9</v>
+      </c>
+      <c r="F12">
+        <v>17.7</v>
+      </c>
+      <c r="G12">
+        <v>7.05</v>
+      </c>
+      <c r="H12" s="9">
+        <v>26.8</v>
+      </c>
+      <c r="I12" s="64">
+        <v>13.6002631578947</v>
+      </c>
+      <c r="J12" s="64">
+        <v>13.0713381995134</v>
+      </c>
+      <c r="K12" s="66">
+        <v>4.5957771759546397E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="79"/>
+      <c r="B13" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>26.2</v>
+      </c>
+      <c r="E13">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="F13">
+        <v>36.844999999999999</v>
+      </c>
+      <c r="G13">
+        <v>22.9</v>
+      </c>
+      <c r="H13" s="9">
+        <v>41.9</v>
+      </c>
+      <c r="I13" s="69">
+        <v>32.046705539358598</v>
+      </c>
+      <c r="J13" s="69">
+        <v>33.739514563106802</v>
+      </c>
+      <c r="K13" s="93" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="79"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>28.827500000000001</v>
+      </c>
+      <c r="E14">
+        <v>33.9</v>
+      </c>
+      <c r="F14">
+        <v>37.772500000000001</v>
+      </c>
+      <c r="G14">
+        <v>13.66</v>
+      </c>
+      <c r="H14" s="9">
+        <v>44.1</v>
+      </c>
+      <c r="I14" s="69">
+        <v>32.046705539358598</v>
+      </c>
+      <c r="J14" s="69">
+        <v>33.739514563106802</v>
+      </c>
+      <c r="K14" s="93"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="79"/>
+      <c r="B15" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D8">
-        <v>144.36000000000001</v>
-      </c>
-      <c r="E8">
-        <v>164</v>
-      </c>
-      <c r="F8">
-        <v>175</v>
-      </c>
-      <c r="G8">
-        <v>130.5</v>
-      </c>
-      <c r="H8" s="9">
-        <v>177</v>
-      </c>
-      <c r="I8" s="55">
-        <v>162.44821705426401</v>
-      </c>
-      <c r="J8" s="55">
-        <v>167.47703703703701</v>
-      </c>
-      <c r="K8" s="55">
-        <v>1.6205747525596199E-6</v>
-      </c>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="3" t="s">
+      <c r="D15">
+        <v>62.3</v>
+      </c>
+      <c r="E15">
+        <v>69.83</v>
+      </c>
+      <c r="F15">
+        <v>74.444999999999993</v>
+      </c>
+      <c r="G15">
+        <v>54.6</v>
+      </c>
+      <c r="H15" s="9">
+        <v>80</v>
+      </c>
+      <c r="I15" s="69">
+        <v>69.530320699708497</v>
+      </c>
+      <c r="J15" s="64">
+        <v>71.312063106796103</v>
+      </c>
+      <c r="K15" s="93" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="80"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9">
-        <v>145.91499999999999</v>
-      </c>
-      <c r="E9">
-        <v>169</v>
-      </c>
-      <c r="F9">
-        <v>180.65</v>
-      </c>
-      <c r="G9">
-        <v>143</v>
-      </c>
-      <c r="H9" s="9">
-        <v>191</v>
-      </c>
-      <c r="I9" s="55">
-        <v>162.44821705426401</v>
-      </c>
-      <c r="J9" s="55">
-        <v>167.47703703703701</v>
-      </c>
-      <c r="K9" s="55">
-        <v>1.6205747525596199E-6</v>
-      </c>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="48" t="s">
+      <c r="D16">
+        <v>65.182500000000005</v>
+      </c>
+      <c r="E16">
+        <v>71.5</v>
+      </c>
+      <c r="F16">
+        <v>76.5</v>
+      </c>
+      <c r="G16">
+        <v>51.9</v>
+      </c>
+      <c r="H16" s="3">
+        <v>79.5</v>
+      </c>
+      <c r="I16" s="69">
+        <v>69.530320699708497</v>
+      </c>
+      <c r="J16" s="65">
+        <v>71.312063106796103</v>
+      </c>
+      <c r="K16" s="94"/>
+    </row>
+    <row r="17" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="8">
-        <v>10</v>
-      </c>
-      <c r="E10" s="8">
-        <v>13.5</v>
-      </c>
-      <c r="F10" s="8">
-        <v>17.647500000000001</v>
-      </c>
-      <c r="G10" s="8">
-        <v>7.1</v>
-      </c>
-      <c r="H10" s="8">
-        <v>23.93</v>
-      </c>
-      <c r="I10" s="54">
-        <v>13.6002631578947</v>
-      </c>
-      <c r="J10" s="54">
-        <v>13.0713381995134</v>
-      </c>
-      <c r="K10" s="58">
-        <v>1.10861488319146E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="45"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="28" t="s">
+      <c r="D17" s="8">
+        <v>22.3</v>
+      </c>
+      <c r="E17" s="8">
+        <v>28</v>
+      </c>
+      <c r="F17" s="8">
+        <v>35</v>
+      </c>
+      <c r="G17" s="8">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="H17" s="8">
+        <v>38.4</v>
+      </c>
+      <c r="I17" s="67">
+        <v>28.176310000000001</v>
+      </c>
+      <c r="J17" s="64">
+        <v>28.107546174142499</v>
+      </c>
+      <c r="K17" s="68">
+        <v>0.78110223387797095</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="72"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D11">
-        <v>9.15</v>
-      </c>
-      <c r="E11">
-        <v>12.9</v>
-      </c>
-      <c r="F11">
-        <v>17.7</v>
-      </c>
-      <c r="G11">
-        <v>7.05</v>
-      </c>
-      <c r="H11" s="9">
-        <v>26.8</v>
-      </c>
-      <c r="I11" s="55">
-        <v>13.6002631578947</v>
-      </c>
-      <c r="J11" s="55">
-        <v>13.0713381995134</v>
-      </c>
-      <c r="K11" s="59">
-        <v>1.10861488319146E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
-      <c r="B12" s="50" t="s">
+      <c r="D18">
+        <v>20.945</v>
+      </c>
+      <c r="E18">
+        <v>28</v>
+      </c>
+      <c r="F18">
+        <v>34.685000000000002</v>
+      </c>
+      <c r="G18">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="H18" s="9">
+        <v>42.3</v>
+      </c>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="66"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="72"/>
+      <c r="B19" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C19" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D12">
-        <v>26.2</v>
-      </c>
-      <c r="E12">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="F12">
-        <v>36.844999999999999</v>
-      </c>
-      <c r="G12">
-        <v>22.9</v>
-      </c>
-      <c r="H12" s="9">
-        <v>41.9</v>
-      </c>
-      <c r="I12" s="60">
-        <v>32.046705539358598</v>
-      </c>
-      <c r="J12" s="60">
-        <v>33.739514563106802</v>
-      </c>
-      <c r="K12" s="59">
-        <v>2.6342277072619602E-19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="28" t="s">
+      <c r="D19">
+        <v>52.13</v>
+      </c>
+      <c r="E19">
+        <v>61.8</v>
+      </c>
+      <c r="F19">
+        <v>68.135000000000005</v>
+      </c>
+      <c r="G19">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="H19" s="9">
+        <v>80.5</v>
+      </c>
+      <c r="I19" s="64">
+        <v>61.495035128805597</v>
+      </c>
+      <c r="J19" s="64">
+        <v>62.095831134564598</v>
+      </c>
+      <c r="K19" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="79"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D13">
-        <v>28.827500000000001</v>
-      </c>
-      <c r="E13">
-        <v>33.9</v>
-      </c>
-      <c r="F13">
-        <v>37.772500000000001</v>
-      </c>
-      <c r="G13">
-        <v>13.66</v>
-      </c>
-      <c r="H13" s="9">
-        <v>44.1</v>
-      </c>
-      <c r="I13" s="60">
-        <v>32.046705539358598</v>
-      </c>
-      <c r="J13" s="60">
-        <v>33.739514563106802</v>
-      </c>
-      <c r="K13" s="59">
-        <v>2.6342277072619602E-19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
-      <c r="B14" s="51" t="s">
+      <c r="D20">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <v>62.3</v>
+      </c>
+      <c r="F20">
+        <v>68.454999999999998</v>
+      </c>
+      <c r="G20">
+        <v>31.6</v>
+      </c>
+      <c r="H20" s="9">
+        <v>73.8</v>
+      </c>
+      <c r="I20" s="64">
+        <v>61.495035128805597</v>
+      </c>
+      <c r="J20" s="64">
+        <v>62.095831134564598</v>
+      </c>
+      <c r="K20" s="66">
+        <v>2.8985319598997999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="79"/>
+      <c r="B21" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D14">
-        <v>62.3</v>
-      </c>
-      <c r="E14">
-        <v>69.83</v>
-      </c>
-      <c r="F14">
-        <v>74.444999999999993</v>
-      </c>
-      <c r="G14">
-        <v>54.6</v>
-      </c>
-      <c r="H14" s="9">
-        <v>80</v>
-      </c>
-      <c r="I14" s="60">
-        <v>69.530320699708497</v>
-      </c>
-      <c r="J14" s="55">
-        <v>71.312063106796103</v>
-      </c>
-      <c r="K14" s="59">
-        <v>3.11342964649108E-14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="3" t="s">
+      <c r="D21">
+        <v>120</v>
+      </c>
+      <c r="E21">
+        <v>129.6</v>
+      </c>
+      <c r="F21">
+        <v>137.345</v>
+      </c>
+      <c r="G21">
+        <v>103.2</v>
+      </c>
+      <c r="H21" s="9">
+        <v>140</v>
+      </c>
+      <c r="I21" s="69">
+        <v>129.138196721311</v>
+      </c>
+      <c r="J21" s="64">
+        <v>128.91445910290199</v>
+      </c>
+      <c r="K21" s="66">
+        <v>0.48402909292805302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="80"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15">
-        <v>65.182500000000005</v>
-      </c>
-      <c r="E15">
-        <v>71.5</v>
-      </c>
-      <c r="F15">
-        <v>76.5</v>
-      </c>
-      <c r="G15">
-        <v>51.9</v>
-      </c>
-      <c r="H15" s="3">
-        <v>79.5</v>
-      </c>
-      <c r="I15" s="60">
-        <v>69.530320699708497</v>
-      </c>
-      <c r="J15" s="57">
-        <v>71.312063106796103</v>
-      </c>
-      <c r="K15" s="59">
-        <v>3.11342964649108E-14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="48" t="s">
+      <c r="D22" s="3">
+        <v>120</v>
+      </c>
+      <c r="E22" s="3">
+        <v>129.4</v>
+      </c>
+      <c r="F22" s="9">
+        <v>136.14150000000001</v>
+      </c>
+      <c r="G22">
+        <v>105.3</v>
+      </c>
+      <c r="H22" s="3">
+        <v>142.6</v>
+      </c>
+      <c r="I22" s="69"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="70"/>
+    </row>
+    <row r="23" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="8">
-        <v>22.3</v>
-      </c>
-      <c r="E16" s="8">
-        <v>28</v>
-      </c>
-      <c r="F16" s="8">
-        <v>35</v>
-      </c>
-      <c r="G16" s="8">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="H16" s="8">
-        <v>38.4</v>
-      </c>
-      <c r="I16" s="54">
-        <v>28.176310000000001</v>
-      </c>
-      <c r="J16" s="55">
-        <v>28.107546174142499</v>
-      </c>
-      <c r="K16" s="58">
-        <v>0.78110223387797095</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="45"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="28" t="s">
+      <c r="D23">
+        <v>10.419499999999999</v>
+      </c>
+      <c r="E23">
+        <v>19.754999999999999</v>
+      </c>
+      <c r="F23" s="8">
+        <v>32.5</v>
+      </c>
+      <c r="G23" s="8">
+        <v>7.13</v>
+      </c>
+      <c r="H23" s="8">
+        <v>41.143333329999997</v>
+      </c>
+      <c r="I23" s="67">
+        <v>19.980257420714299</v>
+      </c>
+      <c r="J23" s="64">
+        <v>20.697463305208299</v>
+      </c>
+      <c r="K23" s="68">
+        <v>0.43730687659225598</v>
+      </c>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="72"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D17">
-        <v>20.945</v>
-      </c>
-      <c r="E17">
-        <v>28</v>
-      </c>
-      <c r="F17">
-        <v>34.685000000000002</v>
-      </c>
-      <c r="G17">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="H17" s="9">
-        <v>42.3</v>
-      </c>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="59"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="45"/>
-      <c r="B18" s="50" t="s">
+      <c r="D24">
+        <v>10.5275</v>
+      </c>
+      <c r="E24">
+        <v>20.59</v>
+      </c>
+      <c r="F24">
+        <v>33.44</v>
+      </c>
+      <c r="G24">
+        <v>7.29</v>
+      </c>
+      <c r="H24" s="9">
+        <v>40.058750000000003</v>
+      </c>
+      <c r="I24" s="64">
+        <v>19.980257420714299</v>
+      </c>
+      <c r="J24" s="64">
+        <v>20.697463305208299</v>
+      </c>
+      <c r="K24" s="66">
+        <v>0.43730687659225598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="72"/>
+      <c r="B25" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C25" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D18">
-        <v>52.13</v>
-      </c>
-      <c r="E18">
-        <v>61.8</v>
-      </c>
-      <c r="F18">
-        <v>68.135000000000005</v>
-      </c>
-      <c r="G18">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="H18" s="9">
-        <v>80.5</v>
-      </c>
-      <c r="I18" s="55">
-        <v>61.495035128805597</v>
-      </c>
-      <c r="J18" s="55">
-        <v>62.095831134564598</v>
-      </c>
-      <c r="K18" s="59">
-        <v>2.8985319598997999E-2</v>
-      </c>
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="28" t="s">
+      <c r="D25">
+        <v>13.67675</v>
+      </c>
+      <c r="E25">
+        <v>29.965</v>
+      </c>
+      <c r="F25">
+        <v>70.95</v>
+      </c>
+      <c r="G25">
+        <v>7.49</v>
+      </c>
+      <c r="H25" s="9">
+        <v>92.575000000000003</v>
+      </c>
+      <c r="I25" s="64">
+        <v>34.6308528837097</v>
+      </c>
+      <c r="J25" s="64">
+        <v>37.053971168548401</v>
+      </c>
+      <c r="K25" s="66">
+        <v>0.47115295738902502</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="79"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D19">
-        <v>55</v>
-      </c>
-      <c r="E19">
-        <v>62.3</v>
-      </c>
-      <c r="F19">
-        <v>68.454999999999998</v>
-      </c>
-      <c r="G19">
-        <v>31.6</v>
-      </c>
-      <c r="H19" s="9">
-        <v>73.8</v>
-      </c>
-      <c r="I19" s="55">
-        <v>61.495035128805597</v>
-      </c>
-      <c r="J19" s="55">
-        <v>62.095831134564598</v>
-      </c>
-      <c r="K19" s="59">
-        <v>2.8985319598997999E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="46"/>
-      <c r="B20" s="51" t="s">
+      <c r="D26">
+        <v>14.488250000000001</v>
+      </c>
+      <c r="E26">
+        <v>32.18</v>
+      </c>
+      <c r="F26">
+        <v>69.816249999999997</v>
+      </c>
+      <c r="G26">
+        <v>12.65</v>
+      </c>
+      <c r="H26" s="9">
+        <v>103.556667</v>
+      </c>
+      <c r="I26" s="64">
+        <v>34.6308528837097</v>
+      </c>
+      <c r="J26" s="64">
+        <v>37.053971168548401</v>
+      </c>
+      <c r="K26" s="66">
+        <v>0.47115295738902502</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="79"/>
+      <c r="B27" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D20">
-        <v>120</v>
-      </c>
-      <c r="E20">
-        <v>129.6</v>
-      </c>
-      <c r="F20">
-        <v>137.345</v>
-      </c>
-      <c r="G20">
-        <v>103.2</v>
-      </c>
-      <c r="H20" s="9">
-        <v>140</v>
-      </c>
-      <c r="I20" s="60">
-        <v>129.138196721311</v>
-      </c>
-      <c r="J20" s="55">
-        <v>128.91445910290199</v>
-      </c>
-      <c r="K20" s="59">
-        <v>0.48402909292805302</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="3" t="s">
+      <c r="D27">
+        <v>41.808500000000002</v>
+      </c>
+      <c r="E27">
+        <v>79</v>
+      </c>
+      <c r="F27">
+        <v>163.73500000000001</v>
+      </c>
+      <c r="G27">
+        <v>38.11</v>
+      </c>
+      <c r="H27" s="9">
+        <v>190</v>
+      </c>
+      <c r="I27" s="64">
+        <v>88.603570949440595</v>
+      </c>
+      <c r="J27" s="64">
+        <v>93.824897517883201</v>
+      </c>
+      <c r="K27" s="66">
+        <v>0.25859645456750502</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="80"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="3">
-        <v>120</v>
-      </c>
-      <c r="E21" s="3">
-        <v>129.4</v>
-      </c>
-      <c r="F21" s="9">
-        <v>136.14150000000001</v>
-      </c>
-      <c r="G21">
-        <v>105.3</v>
-      </c>
-      <c r="H21" s="3">
-        <v>142.6</v>
-      </c>
-      <c r="I21" s="60"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="61"/>
-    </row>
-    <row r="22" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22">
-        <v>10.419499999999999</v>
-      </c>
-      <c r="E22">
-        <v>19.754999999999999</v>
-      </c>
-      <c r="F22" s="8">
-        <v>32.5</v>
-      </c>
-      <c r="G22" s="8">
-        <v>7.13</v>
-      </c>
-      <c r="H22" s="8">
-        <v>41.143333329999997</v>
-      </c>
-      <c r="I22" s="54">
-        <v>19.980257420714299</v>
-      </c>
-      <c r="J22" s="55">
-        <v>20.697463305208299</v>
-      </c>
-      <c r="K22" s="58">
-        <v>0.43730687659225598</v>
-      </c>
-      <c r="L22" s="9"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="45"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23">
-        <v>10.5275</v>
-      </c>
-      <c r="E23">
-        <v>20.59</v>
-      </c>
-      <c r="F23">
-        <v>33.44</v>
-      </c>
-      <c r="G23">
-        <v>7.29</v>
-      </c>
-      <c r="H23" s="9">
-        <v>40.058750000000003</v>
-      </c>
-      <c r="I23" s="55">
-        <v>19.980257420714299</v>
-      </c>
-      <c r="J23" s="55">
-        <v>20.697463305208299</v>
-      </c>
-      <c r="K23" s="59">
-        <v>0.43730687659225598</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="45"/>
-      <c r="B24" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24">
-        <v>13.67675</v>
-      </c>
-      <c r="E24">
-        <v>29.965</v>
-      </c>
-      <c r="F24">
-        <v>70.95</v>
-      </c>
-      <c r="G24">
-        <v>7.49</v>
-      </c>
-      <c r="H24" s="9">
-        <v>92.575000000000003</v>
-      </c>
-      <c r="I24" s="55">
-        <v>34.6308528837097</v>
-      </c>
-      <c r="J24" s="55">
-        <v>37.053971168548401</v>
-      </c>
-      <c r="K24" s="59">
-        <v>0.47115295738902502</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="46"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25">
-        <v>14.488250000000001</v>
-      </c>
-      <c r="E25">
-        <v>32.18</v>
-      </c>
-      <c r="F25">
-        <v>69.816249999999997</v>
-      </c>
-      <c r="G25">
-        <v>12.65</v>
-      </c>
-      <c r="H25" s="9">
-        <v>103.556667</v>
-      </c>
-      <c r="I25" s="55">
-        <v>34.6308528837097</v>
-      </c>
-      <c r="J25" s="55">
-        <v>37.053971168548401</v>
-      </c>
-      <c r="K25" s="59">
-        <v>0.47115295738902502</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
-      <c r="B26" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26">
-        <v>41.808500000000002</v>
-      </c>
-      <c r="E26">
-        <v>79</v>
-      </c>
-      <c r="F26">
-        <v>163.73500000000001</v>
-      </c>
-      <c r="G26">
-        <v>38.11</v>
-      </c>
-      <c r="H26" s="9">
+      <c r="D28" s="9">
+        <v>43.212000000000003</v>
+      </c>
+      <c r="E28" s="9">
+        <v>85.5</v>
+      </c>
+      <c r="F28" s="9">
         <v>190</v>
       </c>
-      <c r="I26" s="55">
+      <c r="G28" s="9">
+        <v>40.15</v>
+      </c>
+      <c r="H28" s="3">
+        <v>238.66666699999999</v>
+      </c>
+      <c r="I28" s="65">
         <v>88.603570949440595</v>
       </c>
-      <c r="J26" s="55">
+      <c r="J28" s="64">
         <v>93.824897517883201</v>
       </c>
-      <c r="K26" s="59">
+      <c r="K28" s="66">
         <v>0.25859645456750502</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="9">
-        <v>43.212000000000003</v>
-      </c>
-      <c r="E27" s="9">
-        <v>85.5</v>
-      </c>
-      <c r="F27" s="9">
-        <v>190</v>
-      </c>
-      <c r="G27" s="9">
-        <v>40.15</v>
-      </c>
-      <c r="H27" s="3">
-        <v>238.66666699999999</v>
-      </c>
-      <c r="I27" s="57">
-        <v>88.603570949440595</v>
-      </c>
-      <c r="J27" s="55">
-        <v>93.824897517883201</v>
-      </c>
-      <c r="K27" s="59">
-        <v>0.25859645456750502</v>
-      </c>
-      <c r="L27" s="9"/>
-    </row>
-    <row r="28" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L30" s="9"/>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="L31" s="9"/>
     </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L32" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
+  <mergeCells count="54">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2271,13 +2304,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2378,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23AC7A9F-3C25-5D41-A126-9879D0594DEC}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2388,7 +2421,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="43" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2398,228 +2431,228 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
     </row>
     <row r="4" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="72"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="84"/>
     </row>
     <row r="5" spans="1:7" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="47" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="77">
+      <c r="B6" s="49">
         <v>-1.36</v>
       </c>
-      <c r="C6" s="77">
+      <c r="C6" s="49">
         <v>0.26800000000000002</v>
       </c>
-      <c r="D6" s="83">
+      <c r="D6" s="55">
         <v>-5.05</v>
       </c>
-      <c r="E6" s="84" t="s">
+      <c r="E6" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="79">
+      <c r="F6" s="51">
         <v>0.97199999999999998</v>
       </c>
-      <c r="G6" s="68"/>
+      <c r="G6" s="43"/>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="77">
+      <c r="B7" s="49">
         <v>1.82</v>
       </c>
-      <c r="C7" s="80">
+      <c r="C7" s="52">
         <v>0.127</v>
       </c>
-      <c r="D7" s="83">
+      <c r="D7" s="55">
         <v>14.32</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="79"/>
-      <c r="G7" s="68"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="43"/>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="77">
+      <c r="B8" s="49">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="C8" s="80">
+      <c r="C8" s="52">
         <v>1.4E-2</v>
       </c>
-      <c r="D8" s="83">
+      <c r="D8" s="55">
         <v>5.44</v>
       </c>
-      <c r="E8" s="84" t="s">
+      <c r="E8" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="79"/>
-      <c r="G8" s="68"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="43"/>
     </row>
     <row r="9" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="85">
+      <c r="B9" s="57">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="C9" s="86">
+      <c r="C9" s="58">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D9" s="88">
+      <c r="D9" s="60">
         <v>-7.97</v>
       </c>
-      <c r="E9" s="87" t="s">
+      <c r="E9" s="59" t="s">
         <v>73</v>
       </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="69"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="44"/>
     </row>
     <row r="11" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="72"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
     </row>
     <row r="12" spans="1:7" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="74" t="s">
+      <c r="D12" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="75" t="s">
+      <c r="F12" s="47" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="77">
+      <c r="B13" s="49">
         <v>-0.998</v>
       </c>
-      <c r="C13" s="77">
+      <c r="C13" s="49">
         <v>0.28399999999999997</v>
       </c>
-      <c r="D13" s="83">
+      <c r="D13" s="55">
         <v>-3.512</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="E13" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="79">
+      <c r="F13" s="51">
         <v>0.96509999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="77">
+      <c r="B14" s="49">
         <v>1.657</v>
       </c>
-      <c r="C14" s="80">
+      <c r="C14" s="52">
         <v>0.13500000000000001</v>
       </c>
-      <c r="D14" s="83">
+      <c r="D14" s="55">
         <v>12.308</v>
       </c>
-      <c r="E14" s="84" t="s">
+      <c r="E14" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="79"/>
+      <c r="F14" s="51"/>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="77">
+      <c r="B15" s="49">
         <v>0.13300000000000001</v>
       </c>
-      <c r="C15" s="80">
+      <c r="C15" s="52">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D15" s="83">
+      <c r="D15" s="55">
         <v>7.7640000000000002</v>
       </c>
-      <c r="E15" s="84" t="s">
+      <c r="E15" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="79"/>
+      <c r="F15" s="51"/>
     </row>
     <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="85">
+      <c r="B16" s="57">
         <v>-0.26800000000000002</v>
       </c>
-      <c r="C16" s="86">
+      <c r="C16" s="58">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D16" s="88">
+      <c r="D16" s="60">
         <v>-7.6580000000000004</v>
       </c>
-      <c r="E16" s="87" t="s">
+      <c r="E16" s="59" t="s">
         <v>73</v>
       </c>
       <c r="F16" s="4"/>
@@ -2653,13 +2686,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2706,10 +2739,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="74" t="s">
         <v>27</v>
       </c>
       <c r="C6" t="s">
@@ -2727,13 +2760,13 @@
       <c r="H6">
         <v>0.13200000000000001</v>
       </c>
-      <c r="J6" s="62">
+      <c r="J6" s="85">
         <v>15.1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="45"/>
-      <c r="B7" s="65"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="14" t="s">
         <v>62</v>
       </c>
@@ -2743,17 +2776,17 @@
       <c r="G7" s="14">
         <v>3.8650000000000002</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="50" t="s">
         <v>73</v>
       </c>
       <c r="I7" s="14">
         <v>3.1579999999999999</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="86"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
-      <c r="B8" s="51" t="s">
+      <c r="A8" s="72"/>
+      <c r="B8" s="75" t="s">
         <v>31</v>
       </c>
       <c r="C8" t="s">
@@ -2771,35 +2804,35 @@
       <c r="H8">
         <v>0.84899999999999998</v>
       </c>
-      <c r="J8" s="63">
+      <c r="J8" s="86">
         <v>13.8</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="82" t="s">
+      <c r="A9" s="72"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82">
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54">
         <v>2.992</v>
       </c>
-      <c r="H9" s="82" t="s">
+      <c r="H9" s="54" t="s">
         <v>91</v>
       </c>
       <c r="I9" s="3">
         <v>4.38</v>
       </c>
-      <c r="J9" s="64"/>
+      <c r="J9" s="87"/>
     </row>
     <row r="10" spans="1:10" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="74" t="s">
         <v>27</v>
       </c>
       <c r="C10" t="s">
@@ -2814,16 +2847,16 @@
       <c r="F10">
         <v>5.3449999999999998</v>
       </c>
-      <c r="H10" s="84" t="s">
+      <c r="H10" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="63">
+      <c r="J10" s="86">
         <v>2.42</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="65"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="88"/>
       <c r="C11" t="s">
         <v>62</v>
       </c>
@@ -2837,11 +2870,11 @@
       <c r="I11">
         <v>4.5830000000000002</v>
       </c>
-      <c r="J11" s="64"/>
+      <c r="J11" s="87"/>
     </row>
     <row r="12" spans="1:10" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
-      <c r="B12" s="65" t="s">
+      <c r="A12" s="72"/>
+      <c r="B12" s="88" t="s">
         <v>31</v>
       </c>
       <c r="C12" t="s">
@@ -2856,38 +2889,38 @@
       <c r="F12" s="42">
         <v>4.891</v>
       </c>
-      <c r="H12" s="84" t="s">
+      <c r="H12" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="J12" s="63">
+      <c r="J12" s="86">
         <v>7.19</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="82" t="s">
+      <c r="A13" s="79"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82">
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54">
         <v>2.6779999999999999</v>
       </c>
-      <c r="H13" s="82" t="s">
+      <c r="H13" s="54" t="s">
         <v>92</v>
       </c>
       <c r="I13" s="3">
         <v>3.859</v>
       </c>
-      <c r="J13" s="64"/>
+      <c r="J13" s="87"/>
     </row>
     <row r="14" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="74" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
@@ -2907,33 +2940,33 @@
         <v>93</v>
       </c>
       <c r="I14" s="8"/>
-      <c r="J14" s="62">
+      <c r="J14" s="85">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="45"/>
-      <c r="B15" s="51"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
       <c r="F15" s="22"/>
-      <c r="G15" s="90">
+      <c r="G15" s="62">
         <v>8.391</v>
       </c>
-      <c r="H15" s="78" t="s">
+      <c r="H15" s="50" t="s">
         <v>73</v>
       </c>
       <c r="I15" s="11">
         <v>4.1390000000000002</v>
       </c>
-      <c r="J15" s="63"/>
+      <c r="J15" s="86"/>
     </row>
     <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="45"/>
-      <c r="B16" s="51" t="s">
+      <c r="A16" s="72"/>
+      <c r="B16" s="75" t="s">
         <v>31</v>
       </c>
       <c r="C16" t="s">
@@ -2953,29 +2986,29 @@
         <v>94</v>
       </c>
       <c r="I16" s="11"/>
-      <c r="J16" s="63">
+      <c r="J16" s="86">
         <v>4.47</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="82" t="s">
+      <c r="A17" s="80"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82">
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54">
         <v>3.0569999999999999</v>
       </c>
-      <c r="H17" s="82" t="s">
+      <c r="H17" s="54" t="s">
         <v>95</v>
       </c>
       <c r="I17" s="3">
         <v>4.7160000000000002</v>
       </c>
-      <c r="J17" s="64"/>
+      <c r="J17" s="87"/>
     </row>
     <row r="18" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -3007,7 +3040,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3024,16 +3057,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -3082,10 +3115,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
@@ -3103,13 +3136,13 @@
       <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="63">
+      <c r="J6" s="86">
         <v>79.599999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="45"/>
-      <c r="B7" s="51"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="75"/>
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -3122,11 +3155,11 @@
       <c r="I7">
         <v>3.2320000000000002</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="86"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
-      <c r="B8" s="51" t="s">
+      <c r="A8" s="72"/>
+      <c r="B8" s="75" t="s">
         <v>20</v>
       </c>
       <c r="C8" t="s">
@@ -3144,13 +3177,13 @@
       <c r="H8" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="63">
+      <c r="J8" s="86">
         <v>70.099999999999994</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="75"/>
       <c r="C9" t="s">
         <v>22</v>
       </c>
@@ -3163,11 +3196,11 @@
       <c r="I9">
         <v>2.7709999999999999</v>
       </c>
-      <c r="J9" s="63"/>
+      <c r="J9" s="86"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="45"/>
-      <c r="B10" s="51" t="s">
+      <c r="A10" s="72"/>
+      <c r="B10" s="75" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -3185,13 +3218,13 @@
       <c r="H10" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="63">
+      <c r="J10" s="86">
         <v>37.6</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
@@ -3207,13 +3240,13 @@
       <c r="I11" s="3">
         <v>2.415</v>
       </c>
-      <c r="J11" s="64"/>
+      <c r="J11" s="87"/>
     </row>
     <row r="12" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
@@ -3231,13 +3264,13 @@
       <c r="H12" t="s">
         <v>63</v>
       </c>
-      <c r="J12" s="63">
+      <c r="J12" s="86">
         <v>63.5</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="45"/>
-      <c r="B13" s="51"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="75"/>
       <c r="C13" t="s">
         <v>22</v>
       </c>
@@ -3251,11 +3284,11 @@
       <c r="I13">
         <v>5.149</v>
       </c>
-      <c r="J13" s="63"/>
+      <c r="J13" s="86"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
-      <c r="B14" s="66" t="s">
+      <c r="A14" s="79"/>
+      <c r="B14" s="89" t="s">
         <v>20</v>
       </c>
       <c r="C14" t="s">
@@ -3273,13 +3306,13 @@
       <c r="H14" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="63">
+      <c r="J14" s="86">
         <v>55.7</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
-      <c r="B15" s="66"/>
+      <c r="A15" s="79"/>
+      <c r="B15" s="89"/>
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -3292,11 +3325,11 @@
       <c r="I15">
         <v>5.2439999999999998</v>
       </c>
-      <c r="J15" s="63"/>
+      <c r="J15" s="86"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
-      <c r="B16" s="51" t="s">
+      <c r="A16" s="79"/>
+      <c r="B16" s="75" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -3314,13 +3347,13 @@
       <c r="H16" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="63">
+      <c r="J16" s="86">
         <v>30.8</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="80"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
@@ -3336,13 +3369,13 @@
       <c r="I17" s="3">
         <v>4.7119999999999997</v>
       </c>
-      <c r="J17" s="64"/>
+      <c r="J17" s="87"/>
     </row>
     <row r="18" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
@@ -3360,13 +3393,13 @@
       <c r="H18" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="63">
+      <c r="J18" s="86">
         <v>78.400000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="45"/>
-      <c r="B19" s="51"/>
+      <c r="A19" s="72"/>
+      <c r="B19" s="75"/>
       <c r="C19" t="s">
         <v>22</v>
       </c>
@@ -3379,11 +3412,11 @@
       <c r="I19">
         <v>5.5090000000000003</v>
       </c>
-      <c r="J19" s="63"/>
+      <c r="J19" s="86"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="46"/>
-      <c r="B20" s="66" t="s">
+      <c r="A20" s="79"/>
+      <c r="B20" s="89" t="s">
         <v>20</v>
       </c>
       <c r="C20" t="s">
@@ -3401,13 +3434,13 @@
       <c r="H20" t="s">
         <v>63</v>
       </c>
-      <c r="J20" s="63">
+      <c r="J20" s="86">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
-      <c r="B21" s="66"/>
+      <c r="A21" s="79"/>
+      <c r="B21" s="89"/>
       <c r="C21" t="s">
         <v>22</v>
       </c>
@@ -3420,11 +3453,11 @@
       <c r="I21">
         <v>3.49</v>
       </c>
-      <c r="J21" s="63"/>
+      <c r="J21" s="86"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="46"/>
-      <c r="B22" s="66" t="s">
+      <c r="A22" s="79"/>
+      <c r="B22" s="89" t="s">
         <v>21</v>
       </c>
       <c r="C22" t="s">
@@ -3442,13 +3475,13 @@
       <c r="H22" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="63">
+      <c r="J22" s="86">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="67"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
@@ -3464,17 +3497,11 @@
       <c r="I23" s="3">
         <v>1</v>
       </c>
-      <c r="J23" s="64"/>
+      <c r="J23" s="87"/>
     </row>
     <row r="24" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="J18:J19"/>
     <mergeCell ref="J20:J21"/>
@@ -3491,6 +3518,12 @@
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="A18:A23"/>
     <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3501,19 +3534,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13ED4145-8C79-4C5B-9CCB-D341CAF22FEA}">
   <dimension ref="A1:G3288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -79103,15 +79136,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC8ED670396C024FAA98AFA812476B31" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d1bee707aa649cf4e55c260e455a28d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="7626d2ff-2312-4551-b3e4-dce0c3c9eecd" xmlns:ns4="ec35cdab-3cb7-48bf-869c-472fc83baa6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7beef39964b21fde8aefb04d1807a203" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -79357,6 +79381,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -79367,24 +79400,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28F35458-DD20-4619-8454-F7428A9AAB6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7626d2ff-2312-4551-b3e4-dce0c3c9eecd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ec35cdab-3cb7-48bf-869c-472fc83baa6a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FB6B83F-860E-4E47-A8D0-874C16A829D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -79404,6 +79419,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28F35458-DD20-4619-8454-F7428A9AAB6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7626d2ff-2312-4551-b3e4-dce0c3c9eecd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ec35cdab-3cb7-48bf-869c-472fc83baa6a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D366AFE-5EF2-46CA-8DB0-CA69774A883C}">
   <ds:schemaRefs>

</xml_diff>